<commit_message>
Dataset update and various tweaks to report styling and report generation.
</commit_message>
<xml_diff>
--- a/datasets/HighlandsMead5-20Data.xlsx
+++ b/datasets/HighlandsMead5-20Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmcgarey/Desktop/Marken Telecom/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D9BC73-A98E-184B-80DA-B8DCFD0547E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB99B3A-EA7B-8F44-8A5C-4B12E32EC1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" xr2:uid="{BE763D09-EEFE-471C-8019-77BB9B4BF485}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="60">
   <si>
     <t>Address</t>
   </si>
@@ -59,12 +59,6 @@
     <t>Address Type</t>
   </si>
   <si>
-    <t>ServiceAddress</t>
-  </si>
-  <si>
-    <t>MailAddress</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -89,15 +83,9 @@
     <t>Garbage Cans</t>
   </si>
   <si>
-    <t>16883 Beaumont Blvd</t>
-  </si>
-  <si>
     <t>Car Repair</t>
   </si>
   <si>
-    <t>16736 Lake Helen Dr.</t>
-  </si>
-  <si>
     <t xml:space="preserve">16767 Lake Helen Dr. </t>
   </si>
   <si>
@@ -122,12 +110,12 @@
     <t>Weeds/Garbage Cans</t>
   </si>
   <si>
-    <t>3175 Beaumont Blvd</t>
-  </si>
-  <si>
     <t>Violation Type</t>
   </si>
   <si>
+    <t xml:space="preserve">Code </t>
+  </si>
+  <si>
     <t>1.8 Vehicle Repair</t>
   </si>
   <si>
@@ -140,35 +128,101 @@
     <t>Tyler Benner</t>
   </si>
   <si>
-    <t>16706 Beaumont Blvd Mead, CO 80542</t>
-  </si>
-  <si>
-    <t>16726 Beaumont Blvd Mead, CO 80542</t>
-  </si>
-  <si>
     <t>Zachary Turner</t>
   </si>
   <si>
     <t>Concenta Lokidong</t>
   </si>
   <si>
-    <t>16743 Beaumont Blvd Mead, CO 80542</t>
-  </si>
-  <si>
     <t>Adan Salomon</t>
   </si>
   <si>
-    <t>16746 Beaumont Blvd Mead, CO 80542</t>
-  </si>
-  <si>
-    <t>Code</t>
+    <t>16683 Beaumont Blvd</t>
+  </si>
+  <si>
+    <t>Courtney Williams</t>
+  </si>
+  <si>
+    <t>Emily Elizabeth Bolks</t>
+  </si>
+  <si>
+    <t>Conrad Christiansen</t>
+  </si>
+  <si>
+    <t>Pranil Lal</t>
+  </si>
+  <si>
+    <t>3157 Beaumont Blvd</t>
+  </si>
+  <si>
+    <t>Howard White</t>
+  </si>
+  <si>
+    <t>Mercedes B. Ramirez Perez</t>
+  </si>
+  <si>
+    <t>Richard Fritche</t>
+  </si>
+  <si>
+    <t>Amy Vigil</t>
+  </si>
+  <si>
+    <t>2.51 Unsightly Conditions</t>
+  </si>
+  <si>
+    <t>Owner or Resident</t>
+  </si>
+  <si>
+    <t>PropertyAddressLine1</t>
+  </si>
+  <si>
+    <t>PropertyCity</t>
+  </si>
+  <si>
+    <t>Mead</t>
+  </si>
+  <si>
+    <t>16767 Lake Helen Blvd.</t>
+  </si>
+  <si>
+    <t>3186 Park St.</t>
+  </si>
+  <si>
+    <t>3205 Beaumont Blvd.</t>
+  </si>
+  <si>
+    <t>PropertyState</t>
+  </si>
+  <si>
+    <t>PropertyZip</t>
+  </si>
+  <si>
+    <t>MailAddressLine1</t>
+  </si>
+  <si>
+    <t>MailCity</t>
+  </si>
+  <si>
+    <t>MailState</t>
+  </si>
+  <si>
+    <t>MailZip</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Alexander Cobb</t>
+  </si>
+  <si>
+    <t>16737 Lake Helen Blvd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +232,20 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -232,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,6 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,15 +644,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6915C7-0B84-4F66-A918-A4BB2E54395E}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.5" customWidth="1"/>
@@ -594,20 +663,22 @@
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33.5" customWidth="1"/>
+    <col min="13" max="13" width="27" customWidth="1"/>
+    <col min="17" max="17" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -624,252 +695,612 @@
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4">
         <v>45797</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2">
+        <v>80542</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" t="s">
+        <v>57</v>
+      </c>
+      <c r="T2">
+        <v>80542</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4">
         <v>45797</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3">
+        <v>80542</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T3">
+        <v>80542</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
       </c>
       <c r="C4" s="4">
         <v>45797</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="M4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4">
+        <v>80542</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4">
+        <v>80542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="4">
         <v>45797</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P5">
+        <v>80542</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>12</v>
+      </c>
+      <c r="R5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" t="s">
+        <v>57</v>
+      </c>
+      <c r="T5">
+        <v>80542</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>33</v>
       </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4">
         <v>45797</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" t="s">
+        <v>57</v>
+      </c>
+      <c r="P6">
+        <v>80524</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" t="s">
+        <v>57</v>
+      </c>
+      <c r="T6">
+        <v>80524</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4">
         <v>45797</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" t="s">
+        <v>57</v>
+      </c>
+      <c r="P7">
+        <v>80524</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" t="s">
+        <v>47</v>
+      </c>
+      <c r="S7" t="s">
+        <v>57</v>
+      </c>
+      <c r="T7">
+        <v>80524</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4">
         <v>45797</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" t="s">
+        <v>57</v>
+      </c>
+      <c r="P8">
+        <v>80524</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" t="s">
+        <v>47</v>
+      </c>
+      <c r="S8" t="s">
+        <v>57</v>
+      </c>
+      <c r="T8">
+        <v>80524</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4">
         <v>45797</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" t="s">
+        <v>57</v>
+      </c>
+      <c r="P9">
+        <v>80524</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>49</v>
+      </c>
+      <c r="R9" t="s">
+        <v>47</v>
+      </c>
+      <c r="S9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T9">
+        <v>80524</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4">
         <v>45797</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" t="s">
+        <v>57</v>
+      </c>
+      <c r="P10">
+        <v>80524</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" t="s">
+        <v>47</v>
+      </c>
+      <c r="S10" t="s">
+        <v>57</v>
+      </c>
+      <c r="T10">
+        <v>80524</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4">
         <v>45797</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>47</v>
+      </c>
+      <c r="O11" t="s">
+        <v>57</v>
+      </c>
+      <c r="P11">
+        <v>80524</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>20</v>
+      </c>
+      <c r="R11" t="s">
+        <v>47</v>
+      </c>
+      <c r="S11" t="s">
+        <v>57</v>
+      </c>
+      <c r="T11">
+        <v>80524</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C12" s="4">
         <v>45797</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="M12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P12">
+        <v>80524</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>21</v>
+      </c>
+      <c r="R12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S12" t="s">
+        <v>57</v>
+      </c>
+      <c r="T12">
+        <v>80524</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4">
         <v>45797</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13" t="s">
+        <v>50</v>
+      </c>
+      <c r="N13" t="s">
+        <v>47</v>
+      </c>
+      <c r="O13" t="s">
+        <v>57</v>
+      </c>
+      <c r="P13">
+        <v>80524</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>50</v>
+      </c>
+      <c r="R13" t="s">
+        <v>47</v>
+      </c>
+      <c r="S13" t="s">
+        <v>57</v>
+      </c>
+      <c r="T13">
+        <v>80524</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C14" s="4">
         <v>45797</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" t="s">
+        <v>47</v>
+      </c>
+      <c r="O14" t="s">
+        <v>57</v>
+      </c>
+      <c r="P14">
+        <v>80542</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>38</v>
+      </c>
+      <c r="R14" t="s">
+        <v>47</v>
+      </c>
+      <c r="S14" t="s">
+        <v>57</v>
+      </c>
+      <c r="T14">
+        <v>80542</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C15" s="4">
         <v>45797</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="22" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="M15" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" t="s">
+        <v>47</v>
+      </c>
+      <c r="O15" t="s">
+        <v>57</v>
+      </c>
+      <c r="P15">
+        <v>80542</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>59</v>
+      </c>
+      <c r="R15" t="s">
+        <v>47</v>
+      </c>
+      <c r="S15" t="s">
+        <v>57</v>
+      </c>
+      <c r="T15">
+        <v>80542</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="22" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>